<commit_message>
New and updated notes
</commit_message>
<xml_diff>
--- a/Labs/Lab05/CS133JS_Lab05_Rubric.xlsx
+++ b/Labs/Lab05/CS133JS_Lab05_Rubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS133JS-CourseMaterials/Labs/Lab05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D2EC45-6ECB-BD4A-988E-1CA12890D00A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AD2965-289A-2E46-A9FB-47822CE92CC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5020" yWindow="1520" windowWidth="17620" windowHeight="12020" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="5020" yWindow="500" windowWidth="17620" windowHeight="14000" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Group A" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Criteria</t>
   </si>
@@ -64,6 +64,24 @@
   </si>
   <si>
     <t>Grading Rubric for Lab 5: Arrays</t>
+  </si>
+  <si>
+    <t>Style and best practices</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>Functions</t>
+  </si>
+  <si>
+    <t>Arrays</t>
+  </si>
+  <si>
+    <t>Grade book, Price list, To-do list</t>
+  </si>
+  <si>
+    <t>Roman to decimal converter, Average of scores, Decimal to roman numeral converter</t>
   </si>
 </sst>
 </file>
@@ -440,121 +458,194 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3216228F-B421-8943-9C69-C9FAC1E7C520}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" customWidth="1"/>
+    <col min="7" max="7" width="1.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:5">
+    <row r="3" spans="1:6">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="4">
-        <v>10</v>
-      </c>
       <c r="E6" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="4">
-        <v>2</v>
-      </c>
       <c r="E8" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="4">
+      <c r="E9" s="4">
+        <v>4</v>
+      </c>
+      <c r="F9" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="4">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="E10" s="4">
+        <v>2</v>
+      </c>
+      <c r="F10" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="4">
+        <v>6</v>
+      </c>
+      <c r="F11" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="4">
-        <v>22</v>
-      </c>
-      <c r="E10" s="4">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+      <c r="E12" s="4">
         <v>7</v>
       </c>
-      <c r="D11" s="4">
-        <v>2</v>
-      </c>
-      <c r="E11" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="F12" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="4">
+        <v>4</v>
+      </c>
+      <c r="F13" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="4">
+        <v>8</v>
+      </c>
+      <c r="F14" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="4">
+        <v>5</v>
+      </c>
+      <c r="F15" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="4">
+        <v>2</v>
+      </c>
+      <c r="F16" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
         <v>3</v>
       </c>
-      <c r="D13">
-        <f>SUM(D6:D11)</f>
+      <c r="E18">
+        <f>SUM(E6:E16)</f>
         <v>50</v>
       </c>
-      <c r="E13">
-        <f>SUM(E6:E11)</f>
+      <c r="F18">
+        <f>SUM(F6:F16)</f>
         <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated notes and rubric
</commit_message>
<xml_diff>
--- a/Labs/Lab05/CS133JS_Lab05_Rubric.xlsx
+++ b/Labs/Lab05/CS133JS_Lab05_Rubric.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS133JS-CourseMaterials/Labs/Lab05/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS133JS-CourseMaterials/Labs/Lab05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1666E1D3-B1C6-D949-93A6-37B5D3D62239}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6252E23-36BB-2D43-A21A-C50F230A0FFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15360" yWindow="500" windowWidth="11280" windowHeight="16460" activeTab="1" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3216228F-B421-8943-9C69-C9FAC1E7C520}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -510,21 +510,23 @@
         <v>11</v>
       </c>
       <c r="E6" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -532,7 +534,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -548,7 +550,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -556,7 +558,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -564,7 +566,7 @@
         <v>16</v>
       </c>
       <c r="E13" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -572,7 +574,7 @@
         <v>15</v>
       </c>
       <c r="E14" s="4">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -580,7 +582,7 @@
         <v>13</v>
       </c>
       <c r="E15" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -597,7 +599,7 @@
       </c>
       <c r="E18">
         <f>SUM(E6:E16)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -627,7 +629,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -675,28 +677,32 @@
         <v>11</v>
       </c>
       <c r="E6" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F6" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -704,10 +710,10 @@
         <v>8</v>
       </c>
       <c r="E9" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -726,10 +732,10 @@
         <v>15</v>
       </c>
       <c r="E11" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -737,10 +743,10 @@
         <v>9</v>
       </c>
       <c r="E12" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -748,10 +754,10 @@
         <v>16</v>
       </c>
       <c r="E13" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -759,10 +765,10 @@
         <v>15</v>
       </c>
       <c r="E14" s="4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F14" s="4">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -770,10 +776,10 @@
         <v>13</v>
       </c>
       <c r="E15" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F15" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -793,11 +799,11 @@
       </c>
       <c r="E18">
         <f>SUM(E6:E16)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F18">
         <f>SUM(F6:F16)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:6">

</xml_diff>

<commit_message>
Updated the rubric and notes
</commit_message>
<xml_diff>
--- a/Labs/Lab05/CS133JS_Lab05_Rubric.xlsx
+++ b/Labs/Lab05/CS133JS_Lab05_Rubric.xlsx
@@ -1,32 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS133JS-CourseMaterials/Labs/Lab05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6252E23-36BB-2D43-A21A-C50F230A0FFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4151F5-153F-E449-AD44-7FB0D5507050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="500" windowWidth="11280" windowHeight="16460" activeTab="1" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
+    <workbookView xWindow="60" yWindow="3880" windowWidth="15220" windowHeight="17480" activeTab="1" xr2:uid="{9702CE45-50CE-F14F-802C-E5FE921247A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Grade" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>Criteria</t>
   </si>
@@ -61,9 +72,6 @@
     <t>All Groups (A, B, and C)</t>
   </si>
   <si>
-    <t>Repetition exercises</t>
-  </si>
-  <si>
     <t>Grading Rubric for Lab 5: Arrays</t>
   </si>
   <si>
@@ -89,6 +97,18 @@
   </si>
   <si>
     <t>Review  with completed "Prod." column</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Array exercises</t>
+  </si>
+  <si>
+    <t>Excellent work!</t>
+  </si>
+  <si>
+    <t>Here's the grade breakdown:</t>
   </si>
 </sst>
 </file>
@@ -145,12 +165,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,7 +499,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E16"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -480,7 +511,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -507,9 +538,9 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4">
+        <v>21</v>
+      </c>
+      <c r="E6">
         <v>8</v>
       </c>
     </row>
@@ -517,7 +548,7 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7">
         <v>0</v>
       </c>
     </row>
@@ -525,7 +556,7 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8">
         <v>1</v>
       </c>
     </row>
@@ -533,23 +564,23 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="4">
+        <v>13</v>
+      </c>
+      <c r="E10">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="4">
+        <v>14</v>
+      </c>
+      <c r="E11">
         <v>5</v>
       </c>
     </row>
@@ -557,31 +588,31 @@
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="4">
+        <v>15</v>
+      </c>
+      <c r="E13">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="4">
+        <v>14</v>
+      </c>
+      <c r="E14">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="4">
+        <v>12</v>
+      </c>
+      <c r="E15">
         <v>4</v>
       </c>
     </row>
@@ -589,7 +620,7 @@
       <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16">
         <v>2</v>
       </c>
     </row>
@@ -607,7 +638,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -615,7 +646,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -626,10 +657,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5839EC90-C7F0-3A4B-8678-BE197ECC720E}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -639,190 +670,229 @@
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="5.6640625" customWidth="1"/>
     <col min="7" max="7" width="1.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" ht="17">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="2" t="s">
+      <c r="H5" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7">
         <v>8</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F7">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="2" t="s">
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="4">
-        <v>0</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="4">
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9">
         <v>1</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F9">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E10">
         <v>3</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F10">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="B10" t="s">
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="4">
-        <v>2</v>
-      </c>
-      <c r="F10" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="4">
+      <c r="E12">
         <v>5</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F12">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E13">
         <v>6</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F13">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="4">
-        <v>3</v>
-      </c>
-      <c r="F13" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8">
       <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15">
         <v>6</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F15">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="4">
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16">
         <v>4</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F16">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="4">
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17">
         <v>2</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
         <v>3</v>
       </c>
-      <c r="E18">
-        <f>SUM(E6:E16)</f>
+      <c r="E19">
+        <f>SUM(E7:E17)</f>
         <v>40</v>
       </c>
-      <c r="F18">
-        <f>SUM(F6:F16)</f>
+      <c r="F19">
+        <f>SUM(F7:F17)</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20">
+      <c r="H19" s="5"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
         <v>1</v>
       </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22">
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
         <v>2</v>
       </c>
-      <c r="B22" t="s">
-        <v>17</v>
+      <c r="B23" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A3:H3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>